<commit_message>
modified: check consistency of input projects
</commit_message>
<xml_diff>
--- a/outputs/Portfolio_solutions.xlsx
+++ b/outputs/Portfolio_solutions.xlsx
@@ -559,7 +559,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4, 5</t>
+          <t>4; 5</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13, 14</t>
+          <t>10; 11; 12; 13; 14</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13, 29</t>
+          <t>10; 11; 12; 13; 29</t>
         </is>
       </c>
     </row>
@@ -805,7 +805,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13</t>
+          <t>10; 11; 12; 13</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>14, 29, 54</t>
+          <t>14; 29; 54</t>
         </is>
       </c>
     </row>
@@ -882,7 +882,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -923,7 +923,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -964,12 +964,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>14, 15, 16, 29, 30, 31, 42, 43, 41</t>
+          <t>14; 15; 16; 29; 30; 31; 42; 43; 41</t>
         </is>
       </c>
     </row>
@@ -1005,12 +1005,12 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>7, 10, 13</t>
+          <t>7; 10; 13</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>15, 23</t>
+          <t>15; 23</t>
         </is>
       </c>
     </row>
@@ -1046,12 +1046,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>13, 14</t>
+          <t>13; 14</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>17, 18, 19, 20, 21, 16</t>
+          <t>17; 18; 19; 20; 21; 16</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>13, 15</t>
+          <t>13; 15</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>15, 16</t>
+          <t>15; 16</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>15, 17</t>
+          <t>15; 17</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>15, 18</t>
+          <t>15; 18</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>15, 20</t>
+          <t>15; 20</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>22, 14</t>
+          <t>22; 14</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>24, 19</t>
+          <t>24; 19</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>27, 28</t>
+          <t>27; 28</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>26, 27</t>
+          <t>26; 27</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>8, 10, 13</t>
+          <t>8; 10; 13</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1661,12 +1661,12 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>13, 29</t>
+          <t>13; 29</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>32, 31, 33</t>
+          <t>32; 31; 33</t>
         </is>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>13, 30</t>
+          <t>13; 30</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1743,12 +1743,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>30, 31</t>
+          <t>30; 31</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>34, 35, 36FC+8</t>
+          <t>34; 35; 36FC+8</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>34, 32, 33</t>
+          <t>34; 32; 33</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>36, 35</t>
+          <t>36; 35</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>39, 40</t>
+          <t>39; 40</t>
         </is>
       </c>
     </row>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>41, 53</t>
+          <t>41; 53</t>
         </is>
       </c>
     </row>
@@ -2112,12 +2112,12 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>40, 13</t>
+          <t>40; 13</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>42, 46, 47</t>
+          <t>42; 46; 47</t>
         </is>
       </c>
     </row>
@@ -2153,12 +2153,12 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>13, 41</t>
+          <t>13; 41</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>43, 45FC+5, 47</t>
+          <t>43; 45FC+5; 47</t>
         </is>
       </c>
     </row>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>13, 42</t>
+          <t>13; 42</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>41, 44</t>
+          <t>41; 44</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>41, 42</t>
+          <t>41; 42</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>46, 45, 47</t>
+          <t>46; 45; 47</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>50, 51, 52FC+2</t>
+          <t>50; 51; 52FC+2</t>
         </is>
       </c>
     </row>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>28, 40, 52, 39, 50, 51</t>
+          <t>28; 40; 52; 39; 50; 51</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>10, 11, 12, 53</t>
+          <t>10; 11; 12; 53</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>4, 55</t>
+          <t>4; 55</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4, 5</t>
+          <t>4; 5</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>7, 8FC+5</t>
+          <t>7; 8FC+5</t>
         </is>
       </c>
     </row>
@@ -3195,12 +3195,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>7, 8</t>
+          <t>7; 8</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13FC+20, 14FC+35, 15</t>
+          <t>10; 11; 12; 13FC+20; 14FC+35; 15</t>
         </is>
       </c>
     </row>
@@ -3364,7 +3364,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>17, 18, 19, 20, 21, 22, 23, 24, 25, 26</t>
+          <t>17; 18; 19; 20; 21; 22; 23; 24; 25; 26</t>
         </is>
       </c>
     </row>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>27, 28, 29</t>
+          <t>27; 28; 29</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29</t>
+          <t>16; 17; 18; 19; 20; 21; 22; 23; 24; 25; 26; 27; 28; 29</t>
         </is>
       </c>
     </row>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>10, 11, 12, 15</t>
+          <t>10; 11; 12; 15</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -3523,7 +3523,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>13, 15, 16</t>
+          <t>13; 15; 16</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -3564,12 +3564,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>13, 15, 17</t>
+          <t>13; 15; 17</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>19, 20</t>
+          <t>19; 20</t>
         </is>
       </c>
     </row>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>13, 15, 18</t>
+          <t>13; 15; 18</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>13, 15, 18, 19</t>
+          <t>13; 15; 18; 19</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -3687,7 +3687,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>13, 15, 20</t>
+          <t>13; 15; 20</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>13, 15, 21</t>
+          <t>13; 15; 21</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -3769,12 +3769,12 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>13, 15, 22</t>
+          <t>13; 15; 22</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>24, 27</t>
+          <t>24; 27</t>
         </is>
       </c>
     </row>
@@ -3810,12 +3810,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>13, 15, 23</t>
+          <t>13; 15; 23</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>25, 26, 27</t>
+          <t>25; 26; 27</t>
         </is>
       </c>
     </row>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>13, 15, 24</t>
+          <t>13; 15; 24</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>13, 15, 24</t>
+          <t>13; 15; 24</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -3933,7 +3933,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>14, 15, 23, 24, 25, 26</t>
+          <t>14; 15; 23; 24; 25; 26</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>14, 15, 27</t>
+          <t>14; 15; 27</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>14, 15, 28</t>
+          <t>14; 15; 28</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>32, 4</t>
+          <t>32; 4</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4, 5</t>
+          <t>4; 5</t>
         </is>
       </c>
     </row>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>6FC+5, 8</t>
+          <t>6FC+5; 8</t>
         </is>
       </c>
     </row>
@@ -4606,12 +4606,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>7, 5</t>
+          <t>7; 5</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>9, 13</t>
+          <t>9; 13</t>
         </is>
       </c>
     </row>
@@ -4652,7 +4652,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>14, 26, 22, 10</t>
+          <t>14; 26; 22; 10</t>
         </is>
       </c>
     </row>
@@ -4693,7 +4693,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>30, 31, 32, 11</t>
+          <t>30; 31; 32; 11</t>
         </is>
       </c>
     </row>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>14, 12</t>
+          <t>14; 12</t>
         </is>
       </c>
     </row>
@@ -4852,7 +4852,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>11, 12, 9</t>
+          <t>11; 12; 9</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -5180,7 +5180,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>9, 21</t>
+          <t>9; 21</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -5267,7 +5267,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>25, 30</t>
+          <t>25; 30</t>
         </is>
       </c>
     </row>
@@ -5308,7 +5308,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>26, 30</t>
+          <t>26; 30</t>
         </is>
       </c>
     </row>
@@ -5344,7 +5344,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>9, 25</t>
+          <t>9; 25</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -5472,7 +5472,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>30, 31</t>
+          <t>30; 31</t>
         </is>
       </c>
     </row>
@@ -5508,7 +5508,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>10, 29, 25, 24</t>
+          <t>10; 29; 25; 24</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -5549,12 +5549,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>30, 10, 29</t>
+          <t>30; 10; 29</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>32, 33</t>
+          <t>32; 33</t>
         </is>
       </c>
     </row>
@@ -5590,12 +5590,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>31, 10</t>
+          <t>31; 10</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>34, 33</t>
+          <t>34; 33</t>
         </is>
       </c>
     </row>
@@ -5631,7 +5631,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>31, 32</t>
+          <t>31; 32</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>33, 32</t>
+          <t>33; 32</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -5754,7 +5754,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>13, 35</t>
+          <t>13; 35</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>37, 4</t>
+          <t>37; 4</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -6063,7 +6063,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4, 5</t>
+          <t>4; 5</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
     </row>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13, 14</t>
+          <t>10; 11; 12; 13; 14</t>
         </is>
       </c>
     </row>
@@ -6268,7 +6268,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13, 29</t>
+          <t>10; 11; 12; 13; 29</t>
         </is>
       </c>
     </row>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13</t>
+          <t>10; 11; 12; 13</t>
         </is>
       </c>
     </row>
@@ -6345,12 +6345,12 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>14, 29, 54</t>
+          <t>14; 29; 54</t>
         </is>
       </c>
     </row>
@@ -6386,7 +6386,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -6427,7 +6427,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -6468,12 +6468,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>7, 8, 9</t>
+          <t>7; 8; 9</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>14, 15, 16, 29, 30, 31, 42, 43, 41</t>
+          <t>14; 15; 16; 29; 30; 31; 42; 43; 41</t>
         </is>
       </c>
     </row>
@@ -6509,12 +6509,12 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>7, 10, 13</t>
+          <t>7; 10; 13</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>15, 23</t>
+          <t>15; 23</t>
         </is>
       </c>
     </row>
@@ -6550,12 +6550,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>13, 14</t>
+          <t>13; 14</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>17, 18, 19, 20, 21, 16</t>
+          <t>17; 18; 19; 20; 21; 16</t>
         </is>
       </c>
     </row>
@@ -6591,7 +6591,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>13, 15</t>
+          <t>13; 15</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -6632,7 +6632,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>15, 16</t>
+          <t>15; 16</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -6673,7 +6673,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>15, 17</t>
+          <t>15; 17</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -6714,7 +6714,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>15, 18</t>
+          <t>15; 18</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -6796,7 +6796,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>15, 20</t>
+          <t>15; 20</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -6878,7 +6878,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>22, 14</t>
+          <t>22; 14</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -6960,7 +6960,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>24, 19</t>
+          <t>24; 19</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -7006,7 +7006,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>27, 28</t>
+          <t>27; 28</t>
         </is>
       </c>
     </row>
@@ -7083,7 +7083,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>26, 27</t>
+          <t>26; 27</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -7124,7 +7124,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>8, 10, 13</t>
+          <t>8; 10; 13</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -7165,12 +7165,12 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>13, 29</t>
+          <t>13; 29</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>32, 31, 33</t>
+          <t>32; 31; 33</t>
         </is>
       </c>
     </row>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>13, 30</t>
+          <t>13; 30</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -7247,12 +7247,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>30, 31</t>
+          <t>30; 31</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>34, 35, 36FC+8</t>
+          <t>34; 35; 36FC+8</t>
         </is>
       </c>
     </row>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>34, 32, 33</t>
+          <t>34; 32; 33</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -7452,7 +7452,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>36, 35</t>
+          <t>36; 35</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -7498,7 +7498,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>39, 40</t>
+          <t>39; 40</t>
         </is>
       </c>
     </row>
@@ -7580,7 +7580,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>41, 53</t>
+          <t>41; 53</t>
         </is>
       </c>
     </row>
@@ -7616,12 +7616,12 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>40, 13</t>
+          <t>40; 13</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>42, 46, 47</t>
+          <t>42; 46; 47</t>
         </is>
       </c>
     </row>
@@ -7657,12 +7657,12 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>13, 41</t>
+          <t>13; 41</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>43, 45FC+5, 47</t>
+          <t>43; 45FC+5; 47</t>
         </is>
       </c>
     </row>
@@ -7698,7 +7698,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>13, 42</t>
+          <t>13; 42</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -7821,7 +7821,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>41, 44</t>
+          <t>41; 44</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -7862,7 +7862,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>41, 42</t>
+          <t>41; 42</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -7903,7 +7903,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>46, 45, 47</t>
+          <t>46; 45; 47</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -7949,7 +7949,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>50, 51, 52FC+2</t>
+          <t>50; 51; 52FC+2</t>
         </is>
       </c>
     </row>
@@ -8108,7 +8108,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>28, 40, 52, 39, 50, 51</t>
+          <t>28; 40; 52; 39; 50; 51</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -8149,7 +8149,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>10, 11, 12, 53</t>
+          <t>10; 11; 12; 53</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>4, 55</t>
+          <t>4; 55</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
@@ -8458,7 +8458,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4, 5</t>
+          <t>4; 5</t>
         </is>
       </c>
     </row>
@@ -8581,7 +8581,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>7, 8FC+5</t>
+          <t>7; 8FC+5</t>
         </is>
       </c>
     </row>
@@ -8699,12 +8699,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>7, 8</t>
+          <t>7; 8</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>10, 11, 12, 13FC+20, 14FC+35, 15</t>
+          <t>10; 11; 12; 13FC+20; 14FC+35; 15</t>
         </is>
       </c>
     </row>
@@ -8868,7 +8868,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>17, 18, 19, 20, 21, 22, 23, 24, 25, 26</t>
+          <t>17; 18; 19; 20; 21; 22; 23; 24; 25; 26</t>
         </is>
       </c>
     </row>
@@ -8909,7 +8909,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>27, 28, 29</t>
+          <t>27; 28; 29</t>
         </is>
       </c>
     </row>
@@ -8950,7 +8950,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29</t>
+          <t>16; 17; 18; 19; 20; 21; 22; 23; 24; 25; 26; 27; 28; 29</t>
         </is>
       </c>
     </row>
@@ -8986,7 +8986,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>10, 11, 12, 15</t>
+          <t>10; 11; 12; 15</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -9027,7 +9027,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>13, 15, 16</t>
+          <t>13; 15; 16</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -9068,12 +9068,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>13, 15, 17</t>
+          <t>13; 15; 17</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>19, 20</t>
+          <t>19; 20</t>
         </is>
       </c>
     </row>
@@ -9109,7 +9109,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>13, 15, 18</t>
+          <t>13; 15; 18</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -9150,7 +9150,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>13, 15, 18, 19</t>
+          <t>13; 15; 18; 19</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -9191,7 +9191,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>13, 15, 20</t>
+          <t>13; 15; 20</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -9232,7 +9232,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>13, 15, 21</t>
+          <t>13; 15; 21</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -9273,12 +9273,12 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>13, 15, 22</t>
+          <t>13; 15; 22</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>24, 27</t>
+          <t>24; 27</t>
         </is>
       </c>
     </row>
@@ -9314,12 +9314,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>13, 15, 23</t>
+          <t>13; 15; 23</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>25, 26, 27</t>
+          <t>25; 26; 27</t>
         </is>
       </c>
     </row>
@@ -9355,7 +9355,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>13, 15, 24</t>
+          <t>13; 15; 24</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -9396,7 +9396,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>13, 15, 24</t>
+          <t>13; 15; 24</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -9437,7 +9437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>14, 15, 23, 24, 25, 26</t>
+          <t>14; 15; 23; 24; 25; 26</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -9478,7 +9478,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>14, 15, 27</t>
+          <t>14; 15; 27</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -9519,7 +9519,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>14, 15, 28</t>
+          <t>14; 15; 28</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -9683,7 +9683,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>32, 4</t>
+          <t>32; 4</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -9910,7 +9910,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4, 5</t>
+          <t>4; 5</t>
         </is>
       </c>
     </row>
@@ -9992,7 +9992,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>6FC+5, 8</t>
+          <t>6FC+5; 8</t>
         </is>
       </c>
     </row>
@@ -10110,12 +10110,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>7, 5</t>
+          <t>7; 5</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>9, 13</t>
+          <t>9; 13</t>
         </is>
       </c>
     </row>
@@ -10156,7 +10156,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>14, 26, 22, 10</t>
+          <t>14; 26; 22; 10</t>
         </is>
       </c>
     </row>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>30, 31, 32, 11</t>
+          <t>30; 31; 32; 11</t>
         </is>
       </c>
     </row>
@@ -10238,7 +10238,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>14, 12</t>
+          <t>14; 12</t>
         </is>
       </c>
     </row>
@@ -10356,7 +10356,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>11, 12, 9</t>
+          <t>11; 12; 9</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -10684,7 +10684,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>9, 21</t>
+          <t>9; 21</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -10771,7 +10771,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>25, 30</t>
+          <t>25; 30</t>
         </is>
       </c>
     </row>
@@ -10812,7 +10812,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>26, 30</t>
+          <t>26; 30</t>
         </is>
       </c>
     </row>
@@ -10848,7 +10848,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>9, 25</t>
+          <t>9; 25</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -10976,7 +10976,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>30, 31</t>
+          <t>30; 31</t>
         </is>
       </c>
     </row>
@@ -11012,7 +11012,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>10, 29, 25, 24</t>
+          <t>10; 29; 25; 24</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -11053,12 +11053,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>30, 10, 29</t>
+          <t>30; 10; 29</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>32, 33</t>
+          <t>32; 33</t>
         </is>
       </c>
     </row>
@@ -11094,12 +11094,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>31, 10</t>
+          <t>31; 10</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>34, 33</t>
+          <t>34; 33</t>
         </is>
       </c>
     </row>
@@ -11135,7 +11135,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>31, 32</t>
+          <t>31; 32</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -11176,7 +11176,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>33, 32</t>
+          <t>33; 32</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -11258,7 +11258,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>13, 35</t>
+          <t>13; 35</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -11340,7 +11340,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>37, 4</t>
+          <t>37; 4</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">

</xml_diff>